<commit_message>
fixed empty entry file error
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlad_\PycharmProjects\testwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EF5CC0-77B1-4BD3-B191-B5AEB0DDACE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF428C0-7BC8-450B-BA82-E56CC236B76A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>row1</t>
   </si>
@@ -36,28 +36,7 @@
     <t>row3</t>
   </si>
   <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>vdsvze</t>
-  </si>
-  <si>
-    <t>acxz</t>
-  </si>
-  <si>
-    <t>fsda</t>
-  </si>
-  <si>
-    <t>fsdavsaef</t>
-  </si>
-  <si>
-    <t>hrfnhmu</t>
-  </si>
-  <si>
     <t>row4</t>
-  </si>
-  <si>
-    <t>ghjbjk</t>
   </si>
 </sst>
 </file>
@@ -393,7 +372,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,103 +392,50 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>312321</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>13421</v>
-      </c>
-      <c r="D2" s="4">
-        <v>36141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2.67</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5654</v>
-      </c>
-      <c r="D3" s="4">
-        <v>36141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>67895679</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2017547</v>
-      </c>
-      <c r="D4" s="4">
-        <v>36141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>21800.6</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>2404</v>
-      </c>
-      <c r="D5" s="4">
-        <v>36141</v>
-      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>21323</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5242</v>
-      </c>
-      <c r="D6" s="4">
-        <v>36141</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>156</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>678</v>
-      </c>
-      <c r="D7" s="4">
-        <v>36141</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
-        <v>456</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created function for adding index, added exceptions for exiting when entered arguments causing errors. Created file and directory for tests.
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlad_\PycharmProjects\testwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF428C0-7BC8-450B-BA82-E56CC236B76A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E8B22-4DE0-447B-A8CF-36AA00EA95D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>row1</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>row4</t>
+  </si>
+  <si>
+    <t>dsanjk</t>
+  </si>
+  <si>
+    <t>dsjai</t>
+  </si>
+  <si>
+    <t>asdjkl</t>
+  </si>
+  <si>
+    <t>rjio</t>
   </si>
 </sst>
 </file>
@@ -372,7 +384,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,28 +408,60 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="4"/>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123.4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>41255</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>312432</v>
+      </c>
+      <c r="C3" s="1">
+        <v>412.6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>35897</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>532</v>
+      </c>
+      <c r="C4" s="1">
+        <v>412.42099999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45430</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="D5" s="4">
+        <v>36892</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -439,5 +483,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed possible SQL injection
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlad_\PycharmProjects\testwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E8B22-4DE0-447B-A8CF-36AA00EA95D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801C66D-4257-491B-80E0-B8C062BFE63A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3312" yWindow="2076" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>row1</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>rjio</t>
+  </si>
+  <si>
+    <t>gfd</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +470,9 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
fixed type recognition. fixed type mismatch when updating table. other small fixes
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlad_\PycharmProjects\testwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801C66D-4257-491B-80E0-B8C062BFE63A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C0A8FB-1328-492E-B894-E471A2D2C03C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3312" yWindow="2076" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>rjio</t>
   </si>
   <si>
-    <t>gfd</t>
+    <t>dsa</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>